<commit_message>
Changed year of baptism to year of birth
</commit_message>
<xml_diff>
--- a/storage/app/public/example-user-import.xlsx
+++ b/storage/app/public/example-user-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Projects/SMPW/CartApp/CartApp/storage/app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C22528-196D-E74E-8E56-A86ABBB48DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B71BB5E-48BF-0141-B2F6-A90C764A4F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16060" yWindow="7800" windowWidth="28040" windowHeight="17440" xr2:uid="{0B34BCC2-07DF-6A46-8C83-7DC0EB2B1ECF}"/>
   </bookViews>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>GENDER</t>
-  </si>
-  <si>
-    <t>YEAR OF BAPTISM</t>
   </si>
   <si>
     <t>APPOINTMENT</t>
@@ -105,6 +102,9 @@
 SPOUSE ID: Optional. Used to link a user that already exists in the system to this user
 RESPONSIBLE BROTHER: Inidcates in the system that a user (brother) has been trained to oversee a shift. Allowed values only. true, false.</t>
     </r>
+  </si>
+  <si>
+    <t>YEAR OF BIRTH</t>
   </si>
 </sst>
 </file>
@@ -156,13 +156,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,14 +480,14 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
@@ -499,19 +499,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="251" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -520,32 +520,32 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for is_unrestricted
</commit_message>
<xml_diff>
--- a/storage/app/public/example-user-import.xlsx
+++ b/storage/app/public/example-user-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Projects/SMPW/CartApp/CartApp/storage/app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2C56AA-99A2-A740-A415-4F8C84C8D40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB4F37-1721-8746-95DD-D713FB118F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16060" yWindow="7800" windowWidth="28040" windowHeight="17440" xr2:uid="{0B34BCC2-07DF-6A46-8C83-7DC0EB2B1ECF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>NAME</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>YEAR OF BIRTH</t>
+  </si>
+  <si>
+    <t>IS UNRESTRICTED</t>
   </si>
   <si>
     <r>
@@ -93,17 +96,270 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-NAME: Full Name
-EMAIL: Propely formatted email address
-MOBILE PHONE: In the format 04XXXXXXXX (spaces can be used)
-GENDER: male, female, m or f
-YEAR OF BIRTH: Optional. 4 digit year. Eg: 1985
-APPOINTMENT: Optional. Allowed values only: elder, ministerial servant
-SERVING AS: Optional. Allowed values only: field missionary, special pioneer, bethel family member, regular pioneer, publisher
-MARITAL STATUS: Optional. Allowed values only: single, married, separated, divorced, widowed
-SPOUSE EMAIL: Optional. Used to link spouses together. If a matching email is found, it will attach the users
-SPOUSE ID: Optional. Used to link a user that already exists in the system to this user
-RESPONSIBLE BROTHER: Inidcates in the system that a user (brother) has been trained to oversee a shift. Allowed values only. true, false.</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NAME:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Full Name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EMAIL:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Propely formatted email address
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MOBILE PHONE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> In the format 04XXXXXXXX (spaces can be used)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GENDER:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> male, female, m or f
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YEAR OF BIRTH:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional. 4 digit year. Eg: 1985
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>APPOINTMENT:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional. Allowed values only: elder, ministerial servant
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SERVING AS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional. Allowed values only: field missionary, special pioneer, bethel family member, regular pioneer, publisher
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MARITAL STATUS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional. Allowed values only: single, married, separated, divorced, widowed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SPOUSE EMAIL:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional. Used to link spouses together. If a matching email is found, it will attach the users
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SPOUSE ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional. Used to link a user that already exists in the system to this user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RESPONSIBLE BROTHER:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Inidcates in the system that a user (brother) has been trained to oversee a shift. Allowed values only. TRUE, FALSE.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IS UNRESTRICTED:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TRUE is the default. If set to false (i.e. indicating they're a 'restricted' user), the volunteer cannot self-roster and they cannot see any shifts other than those they've been rostered onto. Allowed values only. TRUE, FALSE.</t>
     </r>
   </si>
 </sst>
@@ -154,15 +410,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47613A88-4579-004E-B3C1-BFF7EDFD278A}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,24 +751,26 @@
     <col min="9" max="9" width="27" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="251" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="281" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -546,11 +803,14 @@
       </c>
       <c r="K2" t="s">
         <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Refine user import logic with create and update tracking
The user import process has been modified to track both user creation and updates. Instead of solely counting the total rows imported, the revised version separately counts the number of newly imported users and the number of updated existing users. Additionally, the default value for the attribute 'is_unrestricted' has been changed from false to true. Lastly, on a minor note, some code refactor for boolean field tidy up has also been included.
</commit_message>
<xml_diff>
--- a/storage/app/public/example-user-import.xlsx
+++ b/storage/app/public/example-user-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Projects/SMPW/CartApp/CartApp/storage/app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB4F37-1721-8746-95DD-D713FB118F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D1A5E0-62C1-E945-9A35-717C4030B148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16060" yWindow="7800" windowWidth="28040" windowHeight="17440" xr2:uid="{0B34BCC2-07DF-6A46-8C83-7DC0EB2B1ECF}"/>
   </bookViews>
@@ -129,17 +129,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>EMAIL:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Propely formatted email address
+      <t xml:space="preserve">EMAIL: Propely formatted email address. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>NOTE, IF AN EMAIL ADDRESS ALREADY EXISTS FOR A USER IN THE SYSTEM, IT WILL UPDATE THAT USER RECORD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -367,7 +388,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -382,6 +403,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -413,11 +441,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,7 +763,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,8 +782,8 @@
     <col min="12" max="12" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="281" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="281" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4"/>

</xml_diff>